<commit_message>
lower() and replace spacebar with _ from dict keys
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -436,43 +436,43 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Game ID</t>
+          <t>game_id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Home</t>
+          <t>home</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Away</t>
+          <t>away</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Home team goals</t>
+          <t>home_team_goals</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Away team goals</t>
+          <t>away_team_goals</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Winner</t>
+          <t>winner</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -540,10 +540,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -552,33 +552,33 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>saipa</t>
+          <t>jyp</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>kookoo</t>
+          <t>hifk</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>saipa</t>
+          <t>jyp</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
         <v>5</v>
       </c>
-      <c r="B5" t="n">
-        <v>6</v>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>2021-09-10</t>
@@ -586,29 +586,29 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>assat</t>
+          <t>saipa</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>sport</t>
+          <t>kookoo</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>assat</t>
+          <t>saipa</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>7</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" t="n">
         <v>8</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
         <v>9</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="n">
         <v>10</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10" t="n">
         <v>11</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="n">
         <v>12</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B12" t="n">
         <v>13</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" t="n">
         <v>14</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>15</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" t="n">
         <v>16</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" t="n">
         <v>18</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="n">
         <v>20</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="n">
         <v>21</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="n">
         <v>22</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="n">
         <v>23</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="n">
         <v>24</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="n">
         <v>25</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B25" t="n">
         <v>26</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B26" t="n">
         <v>27</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>28</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B28" t="n">
         <v>29</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="n">
         <v>30</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="n">
         <v>31</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B33" t="n">
         <v>34</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" t="n">
         <v>35</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35" t="n">
         <v>36</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="n">
         <v>37</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B43" t="n">
         <v>44</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45" t="n">
         <v>46</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="n">
         <v>47</v>
@@ -2002,7 +2002,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>48</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B48" t="n">
         <v>49</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" t="n">
         <v>50</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B50" t="n">
         <v>51</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B53" t="n">
         <v>54</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="n">
         <v>55</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B56" t="n">
         <v>57</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B57" t="n">
         <v>58</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B58" t="n">
         <v>59</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B59" t="n">
         <v>60</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B60" t="n">
         <v>61</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" t="n">
         <v>62</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B63" t="n">
         <v>64</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" t="n">
         <v>65</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B65" t="n">
         <v>66</v>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B66" t="n">
         <v>67</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B67" t="n">
         <v>68</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B69" t="n">
         <v>70</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B70" t="n">
         <v>71</v>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B71" t="n">
         <v>72</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B72" t="n">
         <v>73</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" t="n">
         <v>74</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B75" t="n">
         <v>76</v>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" t="n">
         <v>77</v>
@@ -3022,7 +3022,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="n">
         <v>78</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B78" t="n">
         <v>79</v>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B79" t="n">
         <v>80</v>
@@ -3124,7 +3124,7 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B80" t="n">
         <v>81</v>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B81" t="n">
         <v>82</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B82" t="n">
         <v>83</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B83" t="n">
         <v>84</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B84" t="n">
         <v>85</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B85" t="n">
         <v>86</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="n">
         <v>87</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B87" t="n">
         <v>88</v>
@@ -3430,7 +3430,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B89" t="n">
         <v>90</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B90" t="n">
         <v>91</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B92" t="n">
         <v>93</v>
@@ -3566,7 +3566,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B93" t="n">
         <v>94</v>
@@ -3600,7 +3600,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B94" t="n">
         <v>95</v>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B95" t="n">
         <v>96</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="n">
         <v>97</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B97" t="n">
         <v>98</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" t="n">
         <v>100</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B100" t="n">
         <v>101</v>
@@ -3838,7 +3838,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B101" t="n">
         <v>102</v>
@@ -3872,7 +3872,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B102" t="n">
         <v>103</v>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B103" t="n">
         <v>104</v>
@@ -3974,7 +3974,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B105" t="n">
         <v>106</v>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B106" t="n">
         <v>107</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B107" t="n">
         <v>108</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" t="n">
         <v>109</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B109" t="n">
         <v>110</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B110" t="n">
         <v>111</v>
@@ -4178,7 +4178,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B111" t="n">
         <v>112</v>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B112" t="n">
         <v>113</v>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B113" t="n">
         <v>114</v>
@@ -4280,7 +4280,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B114" t="n">
         <v>115</v>
@@ -4348,7 +4348,7 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B116" t="n">
         <v>117</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B117" t="n">
         <v>118</v>
@@ -4416,7 +4416,7 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B118" t="n">
         <v>119</v>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B120" t="n">
         <v>121</v>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B121" t="n">
         <v>122</v>
@@ -4552,7 +4552,7 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B122" t="n">
         <v>123</v>
@@ -4586,7 +4586,7 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B123" t="n">
         <v>124</v>
@@ -4620,7 +4620,7 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B124" t="n">
         <v>125</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B125" t="n">
         <v>126</v>
@@ -4688,7 +4688,7 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B126" t="n">
         <v>127</v>
@@ -4756,7 +4756,7 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B128" t="n">
         <v>129</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B129" t="n">
         <v>130</v>
@@ -4824,7 +4824,7 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B130" t="n">
         <v>131</v>
@@ -4858,7 +4858,7 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B131" t="n">
         <v>132</v>
@@ -4892,7 +4892,7 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B132" t="n">
         <v>133</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B133" t="n">
         <v>134</v>
@@ -4960,7 +4960,7 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B134" t="n">
         <v>136</v>
@@ -4994,7 +4994,7 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B135" t="n">
         <v>137</v>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B136" t="n">
         <v>138</v>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B137" t="n">
         <v>139</v>
@@ -5096,7 +5096,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B138" t="n">
         <v>140</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B139" t="n">
         <v>141</v>
@@ -5198,7 +5198,7 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B141" t="n">
         <v>143</v>
@@ -5232,7 +5232,7 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B142" t="n">
         <v>144</v>
@@ -5266,7 +5266,7 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B143" t="n">
         <v>145</v>
@@ -5300,7 +5300,7 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B144" t="n">
         <v>146</v>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B145" t="n">
         <v>147</v>
@@ -5368,7 +5368,7 @@
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B146" t="n">
         <v>148</v>
@@ -5402,7 +5402,7 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B147" t="n">
         <v>149</v>
@@ -5470,7 +5470,7 @@
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B149" t="n">
         <v>151</v>
@@ -5504,7 +5504,7 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B150" t="n">
         <v>152</v>
@@ -5538,7 +5538,7 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B151" t="n">
         <v>153</v>
@@ -5572,7 +5572,7 @@
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B152" t="n">
         <v>154</v>
@@ -5606,7 +5606,7 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B153" t="n">
         <v>155</v>
@@ -5640,7 +5640,7 @@
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B154" t="n">
         <v>156</v>
@@ -5674,7 +5674,7 @@
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B155" t="n">
         <v>157</v>
@@ -5708,7 +5708,7 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B156" t="n">
         <v>158</v>
@@ -5742,7 +5742,7 @@
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B157" t="n">
         <v>159</v>
@@ -5776,7 +5776,7 @@
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B158" t="n">
         <v>160</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B159" t="n">
         <v>161</v>
@@ -5844,7 +5844,7 @@
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B160" t="n">
         <v>162</v>
@@ -5878,7 +5878,7 @@
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B161" t="n">
         <v>163</v>
@@ -5912,7 +5912,7 @@
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B162" t="n">
         <v>164</v>
@@ -5946,7 +5946,7 @@
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B163" t="n">
         <v>165</v>
@@ -5980,7 +5980,7 @@
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B164" t="n">
         <v>166</v>
@@ -6014,7 +6014,7 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B165" t="n">
         <v>167</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B166" t="n">
         <v>168</v>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B167" t="n">
         <v>169</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B168" t="n">
         <v>170</v>
@@ -6150,7 +6150,7 @@
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B169" t="n">
         <v>171</v>
@@ -6218,7 +6218,7 @@
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B171" t="n">
         <v>173</v>
@@ -6252,7 +6252,7 @@
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172" t="n">
         <v>174</v>
@@ -6286,7 +6286,7 @@
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B173" t="n">
         <v>175</v>
@@ -6320,7 +6320,7 @@
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B174" t="n">
         <v>176</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B176" t="n">
         <v>178</v>
@@ -6422,7 +6422,7 @@
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B177" t="n">
         <v>179</v>
@@ -6490,7 +6490,7 @@
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B179" t="n">
         <v>182</v>
@@ -6558,7 +6558,7 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B181" t="n">
         <v>184</v>
@@ -6592,7 +6592,7 @@
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B182" t="n">
         <v>185</v>
@@ -6626,7 +6626,7 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B183" t="n">
         <v>186</v>
@@ -6660,7 +6660,7 @@
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184" t="n">
         <v>187</v>
@@ -6694,7 +6694,7 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B185" t="n">
         <v>188</v>
@@ -6728,7 +6728,7 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B186" t="n">
         <v>189</v>
@@ -6762,7 +6762,7 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B187" t="n">
         <v>190</v>
@@ -6796,7 +6796,7 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B188" t="n">
         <v>191</v>
@@ -6830,7 +6830,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B189" t="n">
         <v>192</v>
@@ -6864,7 +6864,7 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B190" t="n">
         <v>193</v>
@@ -6898,7 +6898,7 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B191" t="n">
         <v>194</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B192" t="n">
         <v>195</v>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B193" t="n">
         <v>196</v>
@@ -7000,7 +7000,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B194" t="n">
         <v>197</v>
@@ -7034,7 +7034,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B195" t="n">
         <v>198</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B196" t="n">
         <v>199</v>
@@ -7170,7 +7170,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B199" t="n">
         <v>202</v>
@@ -7204,7 +7204,7 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B200" t="n">
         <v>203</v>
@@ -7238,7 +7238,7 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B201" t="n">
         <v>204</v>
@@ -7272,7 +7272,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B202" t="n">
         <v>205</v>
@@ -7306,7 +7306,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B203" t="n">
         <v>206</v>
@@ -7340,7 +7340,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B204" t="n">
         <v>207</v>
@@ -7374,7 +7374,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B205" t="n">
         <v>208</v>
@@ -7408,7 +7408,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B206" t="n">
         <v>209</v>
@@ -7442,7 +7442,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B207" t="n">
         <v>210</v>
@@ -7476,7 +7476,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B208" t="n">
         <v>211</v>
@@ -7510,7 +7510,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B209" t="n">
         <v>212</v>
@@ -7544,7 +7544,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B210" t="n">
         <v>213</v>
@@ -7680,7 +7680,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B214" t="n">
         <v>217</v>
@@ -7714,7 +7714,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B215" t="n">
         <v>218</v>
@@ -7748,7 +7748,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B216" t="n">
         <v>219</v>
@@ -7782,7 +7782,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B217" t="n">
         <v>220</v>
@@ -7884,7 +7884,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B220" t="n">
         <v>223</v>
@@ -7918,7 +7918,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B221" t="n">
         <v>224</v>
@@ -7952,7 +7952,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B222" t="n">
         <v>225</v>
@@ -7986,7 +7986,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B223" t="n">
         <v>226</v>
@@ -8020,7 +8020,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B224" t="n">
         <v>227</v>
@@ -8054,7 +8054,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B225" t="n">
         <v>229</v>
@@ -8122,7 +8122,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B227" t="n">
         <v>231</v>
@@ -8156,7 +8156,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B228" t="n">
         <v>232</v>
@@ -8190,7 +8190,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B229" t="n">
         <v>233</v>
@@ -8224,7 +8224,7 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B230" t="n">
         <v>235</v>
@@ -8258,7 +8258,7 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B231" t="n">
         <v>236</v>
@@ -8326,7 +8326,7 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B233" t="n">
         <v>239</v>
@@ -8360,7 +8360,7 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B234" t="n">
         <v>240</v>
@@ -8394,7 +8394,7 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B235" t="n">
         <v>241</v>
@@ -8428,7 +8428,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B236" t="n">
         <v>242</v>
@@ -8462,7 +8462,7 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B237" t="n">
         <v>243</v>
@@ -8496,7 +8496,7 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B238" t="n">
         <v>244</v>
@@ -8530,7 +8530,7 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B239" t="n">
         <v>245</v>
@@ -8564,7 +8564,7 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B240" t="n">
         <v>246</v>
@@ -8598,7 +8598,7 @@
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B241" t="n">
         <v>247</v>
@@ -8632,7 +8632,7 @@
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B242" t="n">
         <v>248</v>
@@ -8666,7 +8666,7 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B243" t="n">
         <v>249</v>
@@ -8700,7 +8700,7 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B244" t="n">
         <v>250</v>
@@ -8734,7 +8734,7 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="B245" t="n">
         <v>251</v>
@@ -8802,7 +8802,7 @@
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B247" t="n">
         <v>253</v>
@@ -8836,7 +8836,7 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B248" t="n">
         <v>254</v>
@@ -8870,7 +8870,7 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B249" t="n">
         <v>255</v>
@@ -8904,7 +8904,7 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B250" t="n">
         <v>258</v>
@@ -8938,7 +8938,7 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="B251" t="n">
         <v>259</v>
@@ -8972,7 +8972,7 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B252" t="n">
         <v>260</v>
@@ -9006,7 +9006,7 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B253" t="n">
         <v>262</v>
@@ -9040,7 +9040,7 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B254" t="n">
         <v>264</v>
@@ -9074,7 +9074,7 @@
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B255" t="n">
         <v>267</v>
@@ -9176,7 +9176,7 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B258" t="n">
         <v>271</v>
@@ -9210,7 +9210,7 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B259" t="n">
         <v>273</v>
@@ -9244,7 +9244,7 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B260" t="n">
         <v>274</v>
@@ -9312,7 +9312,7 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B262" t="n">
         <v>278</v>
@@ -9346,7 +9346,7 @@
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B263" t="n">
         <v>279</v>
@@ -9380,7 +9380,7 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B264" t="n">
         <v>280</v>
@@ -9414,7 +9414,7 @@
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="B265" t="n">
         <v>281</v>
@@ -9448,7 +9448,7 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B266" t="n">
         <v>283</v>
@@ -9482,7 +9482,7 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B267" t="n">
         <v>284</v>
@@ -9516,7 +9516,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B268" t="n">
         <v>285</v>
@@ -9550,7 +9550,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B269" t="n">
         <v>286</v>
@@ -9584,7 +9584,7 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B270" t="n">
         <v>288</v>
@@ -9618,7 +9618,7 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B271" t="n">
         <v>289</v>
@@ -9652,7 +9652,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B272" t="n">
         <v>290</v>
@@ -9686,7 +9686,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B273" t="n">
         <v>292</v>
@@ -9720,7 +9720,7 @@
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B274" t="n">
         <v>294</v>
@@ -9822,7 +9822,7 @@
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B277" t="n">
         <v>304</v>
@@ -9856,7 +9856,7 @@
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B278" t="n">
         <v>305</v>
@@ -9890,7 +9890,7 @@
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B279" t="n">
         <v>308</v>
@@ -9958,7 +9958,7 @@
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B281" t="n">
         <v>310</v>
@@ -9992,7 +9992,7 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B282" t="n">
         <v>312</v>
@@ -10026,7 +10026,7 @@
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B283" t="n">
         <v>313</v>
@@ -10060,7 +10060,7 @@
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B284" t="n">
         <v>314</v>
@@ -10162,7 +10162,7 @@
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B287" t="n">
         <v>320</v>
@@ -10196,7 +10196,7 @@
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B288" t="n">
         <v>321</v>
@@ -10230,7 +10230,7 @@
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B289" t="n">
         <v>322</v>
@@ -10264,7 +10264,7 @@
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B290" t="n">
         <v>323</v>
@@ -10298,7 +10298,7 @@
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B291" t="n">
         <v>325</v>
@@ -10332,7 +10332,7 @@
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B292" t="n">
         <v>326</v>
@@ -10366,7 +10366,7 @@
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B293" t="n">
         <v>328</v>
@@ -10400,7 +10400,7 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B294" t="n">
         <v>329</v>
@@ -10434,7 +10434,7 @@
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B295" t="n">
         <v>330</v>
@@ -10468,7 +10468,7 @@
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B296" t="n">
         <v>331</v>
@@ -10536,7 +10536,7 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B298" t="n">
         <v>333</v>
@@ -10570,7 +10570,7 @@
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B299" t="n">
         <v>334</v>
@@ -10604,7 +10604,7 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B300" t="n">
         <v>335</v>
@@ -10638,7 +10638,7 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B301" t="n">
         <v>336</v>
@@ -10672,7 +10672,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B302" t="n">
         <v>337</v>
@@ -10706,7 +10706,7 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B303" t="n">
         <v>338</v>
@@ -10740,7 +10740,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B304" t="n">
         <v>339</v>
@@ -10774,7 +10774,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B305" t="n">
         <v>340</v>
@@ -10808,7 +10808,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B306" t="n">
         <v>341</v>
@@ -10842,7 +10842,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B307" t="n">
         <v>342</v>
@@ -10876,7 +10876,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B308" t="n">
         <v>343</v>
@@ -10910,7 +10910,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="B309" t="n">
         <v>344</v>
@@ -10944,7 +10944,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B310" t="n">
         <v>345</v>
@@ -10978,7 +10978,7 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B311" t="n">
         <v>346</v>
@@ -11012,7 +11012,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B312" t="n">
         <v>347</v>
@@ -11046,7 +11046,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="B313" t="n">
         <v>348</v>
@@ -11080,7 +11080,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B314" t="n">
         <v>349</v>
@@ -11114,7 +11114,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B315" t="n">
         <v>351</v>
@@ -11148,7 +11148,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B316" t="n">
         <v>352</v>
@@ -11182,7 +11182,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B317" t="n">
         <v>353</v>
@@ -11216,7 +11216,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B318" t="n">
         <v>354</v>
@@ -11250,7 +11250,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B319" t="n">
         <v>356</v>
@@ -11284,7 +11284,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B320" t="n">
         <v>359</v>
@@ -11318,7 +11318,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B321" t="n">
         <v>360</v>
@@ -11352,7 +11352,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B322" t="n">
         <v>361</v>
@@ -11386,7 +11386,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B323" t="n">
         <v>362</v>
@@ -11454,7 +11454,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B325" t="n">
         <v>365</v>
@@ -11522,7 +11522,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B327" t="n">
         <v>368</v>
@@ -11590,7 +11590,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B329" t="n">
         <v>370</v>
@@ -11624,7 +11624,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B330" t="n">
         <v>371</v>
@@ -11658,7 +11658,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B331" t="n">
         <v>372</v>
@@ -11692,7 +11692,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B332" t="n">
         <v>373</v>
@@ -11726,7 +11726,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B333" t="n">
         <v>374</v>
@@ -11760,7 +11760,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B334" t="n">
         <v>375</v>
@@ -11794,7 +11794,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B335" t="n">
         <v>377</v>
@@ -11828,7 +11828,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B336" t="n">
         <v>378</v>
@@ -11896,7 +11896,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="B338" t="n">
         <v>380</v>
@@ -11930,7 +11930,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B339" t="n">
         <v>381</v>
@@ -11964,7 +11964,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B340" t="n">
         <v>383</v>
@@ -11998,7 +11998,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B341" t="n">
         <v>384</v>
@@ -12032,7 +12032,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="B342" t="n">
         <v>386</v>
@@ -12066,7 +12066,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B343" t="n">
         <v>387</v>
@@ -12100,7 +12100,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B344" t="n">
         <v>388</v>
@@ -12134,7 +12134,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B345" t="n">
         <v>389</v>
@@ -12168,7 +12168,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B346" t="n">
         <v>390</v>
@@ -12202,7 +12202,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B347" t="n">
         <v>391</v>
@@ -12236,7 +12236,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B348" t="n">
         <v>392</v>
@@ -12270,7 +12270,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B349" t="n">
         <v>393</v>
@@ -12304,7 +12304,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B350" t="n">
         <v>394</v>
@@ -12338,7 +12338,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B351" t="n">
         <v>395</v>
@@ -12372,7 +12372,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B352" t="n">
         <v>396</v>

</xml_diff>